<commit_message>
IN-884 Mark confirmeddate as Complete in mappings in order to add it to validation SQL
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A81D008-99FB-8F42-B828-D7BF45CF8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C219F-48E7-3F4C-A4C6-A35DAC75BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="6220" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21140" yWindow="4240" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D765A69-DF19-B84F-A530-22008AF977F3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -721,7 +721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="C13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1072,8 +1072,8 @@
       <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="15" t="s">
-        <v>66</v>
+      <c r="O11" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>71</v>
@@ -1097,8 +1097,10 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="O12" s="15" t="s">
-        <v>66</v>
+      <c r="H12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="O12" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P12" s="14" t="s">
         <v>70</v>
@@ -1122,7 +1124,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="12" t="s">
         <v>66</v>
       </c>
       <c r="P13" s="14" t="s">
@@ -2587,9 +2589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2949,8 +2951,8 @@
       <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="15" t="s">
-        <v>66</v>
+      <c r="O11" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>71</v>
@@ -2974,8 +2976,8 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="O12" s="15" t="s">
-        <v>66</v>
+      <c r="O12" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P12" s="14" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
IN-884 Add DB validations for Invoices (#454)
* IN-884 Mark confirmeddate as Complete in mappings in order to add it to validation SQL

* IN-884 Add invoice validations

* IN-884 Fix rounding error

* IN-884 Fix datetime conversion in transform schema

* IN-884 Use Money library to convert monetary amounts to decimals and integers

* IN-884 Rebase

* IN-884 Fix invoice API test failure caused by American date format

* IN-884 fix copy&paste error
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A81D008-99FB-8F42-B828-D7BF45CF8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C219F-48E7-3F4C-A4C6-A35DAC75BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="6220" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21140" yWindow="4240" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D765A69-DF19-B84F-A530-22008AF977F3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -721,7 +721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="C13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1072,8 +1072,8 @@
       <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="15" t="s">
-        <v>66</v>
+      <c r="O11" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>71</v>
@@ -1097,8 +1097,10 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="O12" s="15" t="s">
-        <v>66</v>
+      <c r="H12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="O12" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P12" s="14" t="s">
         <v>70</v>
@@ -1122,7 +1124,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="12" t="s">
         <v>66</v>
       </c>
       <c r="P13" s="14" t="s">
@@ -2587,9 +2589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2949,8 +2951,8 @@
       <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="15" t="s">
-        <v>66</v>
+      <c r="O11" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>71</v>
@@ -2974,8 +2976,8 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="O12" s="15" t="s">
-        <v>66</v>
+      <c r="O12" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="P12" s="14" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Add additional GL Codes lookups to invoice spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C219F-48E7-3F4C-A4C6-A35DAC75BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2644A9E-02A7-834E-B4DA-FFF5607ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="4240" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="33600" windowHeight="19900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="103">
   <si>
     <t>table_name</t>
   </si>
@@ -272,6 +272,72 @@
   </si>
   <si>
     <t>Case, Invoice No, Amount, Create</t>
+  </si>
+  <si>
+    <t>7-00-1-53-20</t>
+  </si>
+  <si>
+    <t>7-00-1-53-30</t>
+  </si>
+  <si>
+    <t>7-00-1-53-50</t>
+  </si>
+  <si>
+    <t>7-00-1-55-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-1-55-30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-1-55-50 </t>
+  </si>
+  <si>
+    <t>7-00-1-55-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-53-20 </t>
+  </si>
+  <si>
+    <t>7-00-2-53-30</t>
+  </si>
+  <si>
+    <t>7-00-2-53-50</t>
+  </si>
+  <si>
+    <t>7-00-2-55-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-55-30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-55-50 </t>
+  </si>
+  <si>
+    <t>7-00-2-55-70</t>
+  </si>
+  <si>
+    <t>J-00-1-55-20</t>
+  </si>
+  <si>
+    <t>J-00-1-55-30</t>
+  </si>
+  <si>
+    <t>J-00-1-55-50</t>
+  </si>
+  <si>
+    <t>J-00-1-55-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-00-2-55-20 </t>
+  </si>
+  <si>
+    <t>J-00-2-55-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-00-2-55-50 </t>
+  </si>
+  <si>
+    <t>J-00-2-55-70</t>
   </si>
 </sst>
 </file>
@@ -281,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -328,6 +394,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -379,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -393,7 +464,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,6 +475,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,80 +708,80 @@
     <col min="7" max="7" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="G7" s="14"/>
+      <c r="G7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -793,25 +866,25 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="b">
+      <c r="E2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
@@ -820,23 +893,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
@@ -845,168 +918,168 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="M5" s="14" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="M5" s="13" t="s">
         <v>73</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>58</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="b">
+      <c r="E8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>69</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9" t="b">
+      <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" t="s">
         <v>54</v>
       </c>
@@ -1016,139 +1089,139 @@
       <c r="K9" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="b">
+      <c r="E10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="14"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="b">
+      <c r="E11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="9" t="b">
+      <c r="E12" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="O12" s="12" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="O12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9" t="b">
+      <c r="E13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="O13" s="12" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="O13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="9" t="b">
+      <c r="E14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" t="s">
         <v>54</v>
       </c>
@@ -1160,27 +1233,27 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="9" t="b">
+      <c r="E15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="M15" s="14" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="M15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2589,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
@@ -2663,25 +2736,25 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="b">
+      <c r="E2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
@@ -2690,23 +2763,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
@@ -2715,51 +2788,51 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" t="s">
         <v>54</v>
       </c>
@@ -2770,122 +2843,122 @@
         <v>56</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>74</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="b">
+      <c r="E8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>75</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9" t="b">
+      <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" t="s">
         <v>54</v>
       </c>
@@ -2895,137 +2968,137 @@
       <c r="K9" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="b">
+      <c r="E10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="14"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="b">
+      <c r="E11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="9" t="b">
+      <c r="E12" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="O12" s="12" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="O12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9" t="b">
+      <c r="E13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="O13" s="15" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="O13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="9" t="b">
+      <c r="E14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" t="s">
         <v>54</v>
       </c>
@@ -3037,27 +3110,27 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="9" t="b">
+      <c r="E15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="M15" s="14" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="M15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4467,16 +4540,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="25" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4493,118 +4570,270 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="E5" s="7"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="D5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="A6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="3"/>
+      <c r="A8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B9" s="3"/>
+      <c r="A9" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="3"/>
+      <c r="A10" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="D10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B11" s="3"/>
+      <c r="A11" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B12" s="3"/>
+      <c r="A12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="D12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B13" s="3"/>
+      <c r="A13" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="D13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B14" s="3"/>
+      <c r="A14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B15" s="3"/>
+      <c r="A15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="D15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="D19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="D24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="D25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="D26" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5159,792 +5388,786 @@
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B216" s="3"/>
     </row>
-    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B218" s="3"/>
-    </row>
-    <row r="219" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="220" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="221" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="222" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="223" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="224" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="217" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="218" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="219" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="220" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="221" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="222" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="223" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="224" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="14" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Add additional GL Codes lookups to invoice spreadsheet (#526)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C219F-48E7-3F4C-A4C6-A35DAC75BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2644A9E-02A7-834E-B4DA-FFF5607ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="4240" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="33600" windowHeight="19900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="103">
   <si>
     <t>table_name</t>
   </si>
@@ -272,6 +272,72 @@
   </si>
   <si>
     <t>Case, Invoice No, Amount, Create</t>
+  </si>
+  <si>
+    <t>7-00-1-53-20</t>
+  </si>
+  <si>
+    <t>7-00-1-53-30</t>
+  </si>
+  <si>
+    <t>7-00-1-53-50</t>
+  </si>
+  <si>
+    <t>7-00-1-55-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-1-55-30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-1-55-50 </t>
+  </si>
+  <si>
+    <t>7-00-1-55-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-53-20 </t>
+  </si>
+  <si>
+    <t>7-00-2-53-30</t>
+  </si>
+  <si>
+    <t>7-00-2-53-50</t>
+  </si>
+  <si>
+    <t>7-00-2-55-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-55-30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-00-2-55-50 </t>
+  </si>
+  <si>
+    <t>7-00-2-55-70</t>
+  </si>
+  <si>
+    <t>J-00-1-55-20</t>
+  </si>
+  <si>
+    <t>J-00-1-55-30</t>
+  </si>
+  <si>
+    <t>J-00-1-55-50</t>
+  </si>
+  <si>
+    <t>J-00-1-55-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-00-2-55-20 </t>
+  </si>
+  <si>
+    <t>J-00-2-55-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-00-2-55-50 </t>
+  </si>
+  <si>
+    <t>J-00-2-55-70</t>
   </si>
 </sst>
 </file>
@@ -281,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -328,6 +394,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -379,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -393,7 +464,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,6 +475,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,80 +708,80 @@
     <col min="7" max="7" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="G7" s="14"/>
+      <c r="G7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -793,25 +866,25 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="b">
+      <c r="E2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
@@ -820,23 +893,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
@@ -845,168 +918,168 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="M5" s="14" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="M5" s="13" t="s">
         <v>73</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>58</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="b">
+      <c r="E8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>69</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9" t="b">
+      <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" t="s">
         <v>54</v>
       </c>
@@ -1016,139 +1089,139 @@
       <c r="K9" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="b">
+      <c r="E10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="14"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="b">
+      <c r="E11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="9" t="b">
+      <c r="E12" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="O12" s="12" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="O12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9" t="b">
+      <c r="E13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="O13" s="12" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="O13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="9" t="b">
+      <c r="E14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" t="s">
         <v>54</v>
       </c>
@@ -1160,27 +1233,27 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="9" t="b">
+      <c r="E15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="M15" s="14" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="M15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2589,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
@@ -2663,25 +2736,25 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="b">
+      <c r="E2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
@@ -2690,23 +2763,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
@@ -2715,51 +2788,51 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" t="s">
         <v>54</v>
       </c>
@@ -2770,122 +2843,122 @@
         <v>56</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>74</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="b">
+      <c r="E8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>75</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9" t="b">
+      <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" t="s">
         <v>54</v>
       </c>
@@ -2895,137 +2968,137 @@
       <c r="K9" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="b">
+      <c r="E10" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="14"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9" t="b">
+      <c r="E11" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="9" t="b">
+      <c r="E12" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="O12" s="12" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="O12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9" t="b">
+      <c r="E13" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="O13" s="15" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="O13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="9" t="b">
+      <c r="E14" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" t="s">
         <v>54</v>
       </c>
@@ -3037,27 +3110,27 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="9" t="b">
+      <c r="E15" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="M15" s="14" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="M15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4467,16 +4540,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="25" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4493,118 +4570,270 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="E5" s="7"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="D5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="A6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="3"/>
+      <c r="A8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B9" s="3"/>
+      <c r="A9" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="3"/>
+      <c r="A10" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="D10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B11" s="3"/>
+      <c r="A11" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B12" s="3"/>
+      <c r="A12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="D12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B13" s="3"/>
+      <c r="A13" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="D13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B14" s="3"/>
+      <c r="A14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B15" s="3"/>
+      <c r="A15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="D15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="D19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="D24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="D25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="D26" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5159,792 +5388,786 @@
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B216" s="3"/>
     </row>
-    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B218" s="3"/>
-    </row>
-    <row r="219" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="220" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="221" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="222" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="223" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="224" spans="2:2" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="217" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="218" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="219" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="220" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="221" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="222" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="223" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="224" spans="2:2" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="14" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
IN-1105 Add more GL codes to supervision level mapping; truncate events table in QA
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2644A9E-02A7-834E-B4DA-FFF5607ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BAB7B-0EA3-F545-B243-F7D7BDC8F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="33600" windowHeight="19900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="106">
   <si>
     <t>table_name</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>J-00-2-55-70</t>
+  </si>
+  <si>
+    <t>60-VW510-115151-000-0000</t>
+  </si>
+  <si>
+    <t>60-VW510-115152-000-0000</t>
+  </si>
+  <si>
+    <t>60-VW510-115157-000-0000</t>
   </si>
 </sst>
 </file>
@@ -4543,7 +4552,7 @@
   <dimension ref="A1:E996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4819,13 +4828,28 @@
       <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="16" t="s">
+        <v>104</v>
+      </c>
       <c r="B28" s="3"/>
+      <c r="D28" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="B29" s="3"/>
+      <c r="D29" s="16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3"/>

</xml_diff>

<commit_message>
IN-1105 Add more GL codes to supervision level mapping; truncate events table in QA (#549)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2644A9E-02A7-834E-B4DA-FFF5607ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BAB7B-0EA3-F545-B243-F7D7BDC8F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="33600" windowHeight="19900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="106">
   <si>
     <t>table_name</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>J-00-2-55-70</t>
+  </si>
+  <si>
+    <t>60-VW510-115151-000-0000</t>
+  </si>
+  <si>
+    <t>60-VW510-115152-000-0000</t>
+  </si>
+  <si>
+    <t>60-VW510-115157-000-0000</t>
   </si>
 </sst>
 </file>
@@ -4543,7 +4552,7 @@
   <dimension ref="A1:E996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4819,13 +4828,28 @@
       <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="16" t="s">
+        <v>104</v>
+      </c>
       <c r="B28" s="3"/>
+      <c r="D28" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="B29" s="3"/>
+      <c r="D29" s="16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3"/>

</xml_diff>

<commit_message>
IN-1105 Remove trailing spaces from lookup values
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BAB7B-0EA3-F545-B243-F7D7BDC8F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249C575E-F3E8-AC43-BCEA-AEC955C9E004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12960" yWindow="1620" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -286,18 +286,9 @@
     <t>7-00-1-55-20</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-1-55-30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-00-1-55-50 </t>
-  </si>
-  <si>
     <t>7-00-1-55-70</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-2-53-20 </t>
-  </si>
-  <si>
     <t>7-00-2-53-30</t>
   </si>
   <si>
@@ -307,12 +298,6 @@
     <t>7-00-2-55-20</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-2-55-30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-00-2-55-50 </t>
-  </si>
-  <si>
     <t>7-00-2-55-70</t>
   </si>
   <si>
@@ -328,15 +313,9 @@
     <t>J-00-1-55-70</t>
   </si>
   <si>
-    <t xml:space="preserve">J-00-2-55-20 </t>
-  </si>
-  <si>
     <t>J-00-2-55-30</t>
   </si>
   <si>
-    <t xml:space="preserve">J-00-2-55-50 </t>
-  </si>
-  <si>
     <t>J-00-2-55-70</t>
   </si>
   <si>
@@ -347,6 +326,27 @@
   </si>
   <si>
     <t>60-VW510-115157-000-0000</t>
+  </si>
+  <si>
+    <t>7-00-1-55-30</t>
+  </si>
+  <si>
+    <t>7-00-1-55-50</t>
+  </si>
+  <si>
+    <t>7-00-2-53-20</t>
+  </si>
+  <si>
+    <t>7-00-2-55-30</t>
+  </si>
+  <si>
+    <t>7-00-2-55-50</t>
+  </si>
+  <si>
+    <t>J-00-2-55-20</t>
+  </si>
+  <si>
+    <t>J-00-2-55-50</t>
   </si>
 </sst>
 </file>
@@ -4552,7 +4552,7 @@
   <dimension ref="A1:E996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B9" s="18"/>
       <c r="D9" s="18" t="s">
@@ -4659,7 +4659,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B10" s="18"/>
       <c r="D10" s="18" t="s">
@@ -4669,7 +4669,7 @@
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="18"/>
       <c r="D11" s="18" t="s">
@@ -4679,7 +4679,7 @@
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B12" s="18"/>
       <c r="D12" s="18" t="s">
@@ -4689,7 +4689,7 @@
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" s="18"/>
       <c r="D13" s="18" t="s">
@@ -4699,7 +4699,7 @@
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" s="18"/>
       <c r="D14" s="18" t="s">
@@ -4709,7 +4709,7 @@
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="18"/>
       <c r="D15" s="18" t="s">
@@ -4719,7 +4719,7 @@
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B16" s="18"/>
       <c r="D16" s="18" t="s">
@@ -4729,7 +4729,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B17" s="18"/>
       <c r="D17" s="18" t="s">
@@ -4739,7 +4739,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B18" s="18"/>
       <c r="D18" s="18" t="s">
@@ -4749,7 +4749,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B19" s="18"/>
       <c r="D19" s="18" t="s">
@@ -4759,7 +4759,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B20" s="18"/>
       <c r="D20" s="18" t="s">
@@ -4769,7 +4769,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B21" s="18"/>
       <c r="D21" s="18" t="s">
@@ -4779,7 +4779,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22" s="18"/>
       <c r="D22" s="18" t="s">
@@ -4789,7 +4789,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B23" s="18"/>
       <c r="D23" s="18" t="s">
@@ -4799,7 +4799,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B24" s="18"/>
       <c r="D24" s="18" t="s">
@@ -4809,7 +4809,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B25" s="18"/>
       <c r="D25" s="18" t="s">
@@ -4819,7 +4819,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B26" s="18"/>
       <c r="D26" s="18" t="s">
@@ -4829,13 +4829,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B28" s="3"/>
       <c r="D28" s="16" t="s">
@@ -4844,7 +4844,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B29" s="3"/>
       <c r="D29" s="16" t="s">

</xml_diff>

<commit_message>
IN-1105 Remove trailing spaces from lookup values (#552)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1BAB7B-0EA3-F545-B243-F7D7BDC8F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249C575E-F3E8-AC43-BCEA-AEC955C9E004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12960" yWindow="1620" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -286,18 +286,9 @@
     <t>7-00-1-55-20</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-1-55-30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-00-1-55-50 </t>
-  </si>
-  <si>
     <t>7-00-1-55-70</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-2-53-20 </t>
-  </si>
-  <si>
     <t>7-00-2-53-30</t>
   </si>
   <si>
@@ -307,12 +298,6 @@
     <t>7-00-2-55-20</t>
   </si>
   <si>
-    <t xml:space="preserve">7-00-2-55-30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-00-2-55-50 </t>
-  </si>
-  <si>
     <t>7-00-2-55-70</t>
   </si>
   <si>
@@ -328,15 +313,9 @@
     <t>J-00-1-55-70</t>
   </si>
   <si>
-    <t xml:space="preserve">J-00-2-55-20 </t>
-  </si>
-  <si>
     <t>J-00-2-55-30</t>
   </si>
   <si>
-    <t xml:space="preserve">J-00-2-55-50 </t>
-  </si>
-  <si>
     <t>J-00-2-55-70</t>
   </si>
   <si>
@@ -347,6 +326,27 @@
   </si>
   <si>
     <t>60-VW510-115157-000-0000</t>
+  </si>
+  <si>
+    <t>7-00-1-55-30</t>
+  </si>
+  <si>
+    <t>7-00-1-55-50</t>
+  </si>
+  <si>
+    <t>7-00-2-53-20</t>
+  </si>
+  <si>
+    <t>7-00-2-55-30</t>
+  </si>
+  <si>
+    <t>7-00-2-55-50</t>
+  </si>
+  <si>
+    <t>J-00-2-55-20</t>
+  </si>
+  <si>
+    <t>J-00-2-55-50</t>
   </si>
 </sst>
 </file>
@@ -4552,7 +4552,7 @@
   <dimension ref="A1:E996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B9" s="18"/>
       <c r="D9" s="18" t="s">
@@ -4659,7 +4659,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B10" s="18"/>
       <c r="D10" s="18" t="s">
@@ -4669,7 +4669,7 @@
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="18"/>
       <c r="D11" s="18" t="s">
@@ -4679,7 +4679,7 @@
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B12" s="18"/>
       <c r="D12" s="18" t="s">
@@ -4689,7 +4689,7 @@
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" s="18"/>
       <c r="D13" s="18" t="s">
@@ -4699,7 +4699,7 @@
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" s="18"/>
       <c r="D14" s="18" t="s">
@@ -4709,7 +4709,7 @@
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="18"/>
       <c r="D15" s="18" t="s">
@@ -4719,7 +4719,7 @@
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B16" s="18"/>
       <c r="D16" s="18" t="s">
@@ -4729,7 +4729,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B17" s="18"/>
       <c r="D17" s="18" t="s">
@@ -4739,7 +4739,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B18" s="18"/>
       <c r="D18" s="18" t="s">
@@ -4749,7 +4749,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B19" s="18"/>
       <c r="D19" s="18" t="s">
@@ -4759,7 +4759,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B20" s="18"/>
       <c r="D20" s="18" t="s">
@@ -4769,7 +4769,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B21" s="18"/>
       <c r="D21" s="18" t="s">
@@ -4779,7 +4779,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22" s="18"/>
       <c r="D22" s="18" t="s">
@@ -4789,7 +4789,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B23" s="18"/>
       <c r="D23" s="18" t="s">
@@ -4799,7 +4799,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B24" s="18"/>
       <c r="D24" s="18" t="s">
@@ -4809,7 +4809,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B25" s="18"/>
       <c r="D25" s="18" t="s">
@@ -4819,7 +4819,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B26" s="18"/>
       <c r="D26" s="18" t="s">
@@ -4829,13 +4829,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B28" s="3"/>
       <c r="D28" s="16" t="s">
@@ -4844,7 +4844,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B29" s="3"/>
       <c r="D29" s="16" t="s">

</xml_diff>

<commit_message>
IN-1146 phase 2 prep
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249C575E-F3E8-AC43-BCEA-AEC955C9E004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9744EA-75D7-584C-A8E9-2F36AC1D2D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1620" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="460" windowWidth="33600" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -226,9 +226,6 @@
     <t>NOT MAPPED</t>
   </si>
   <si>
-    <t>CASRECMIGRATION</t>
-  </si>
-  <si>
     <t>finance_invoice_ad</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>J-00-2-55-50</t>
+  </si>
+  <si>
+    <t>CASRECMIGRATION_P2</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>38</v>
@@ -760,15 +760,15 @@
         <v>54</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>38</v>
@@ -783,10 +783,10 @@
         <v>54</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -803,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="C13:O13"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -819,7 +819,7 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="15" width="11.5" customWidth="1"/>
     <col min="16" max="16" width="32.6640625" customWidth="1"/>
   </cols>
@@ -951,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="M5" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="12" t="s">
@@ -1064,7 +1064,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="12" t="s">
@@ -1158,7 +1158,7 @@
         <v>18</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>18</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>66</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="M15" s="13" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>18</v>
@@ -2671,9 +2671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2821,7 +2821,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -2910,7 +2910,7 @@
         <v>58</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M7" s="2"/>
       <c r="O7" s="12" t="s">
@@ -2943,7 +2943,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="12" t="s">
@@ -3037,7 +3037,7 @@
         <v>18</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3062,7 +3062,7 @@
         <v>18</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3087,7 +3087,7 @@
         <v>66</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3137,7 +3137,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="M15" s="13" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>18</v>
@@ -4551,7 +4551,7 @@
   </sheetPr>
   <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="18"/>
       <c r="D5" s="18" t="s">
@@ -4619,7 +4619,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="18"/>
       <c r="D6" s="18" t="s">
@@ -4629,7 +4629,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="18"/>
       <c r="D7" s="18" t="s">
@@ -4639,7 +4639,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="18"/>
       <c r="D8" s="18" t="s">
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="18"/>
       <c r="D9" s="18" t="s">
@@ -4659,7 +4659,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="18"/>
       <c r="D10" s="18" t="s">
@@ -4669,7 +4669,7 @@
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="18"/>
       <c r="D11" s="18" t="s">
@@ -4679,7 +4679,7 @@
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="18"/>
       <c r="D12" s="18" t="s">
@@ -4689,7 +4689,7 @@
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="18"/>
       <c r="D13" s="18" t="s">
@@ -4699,7 +4699,7 @@
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="18"/>
       <c r="D14" s="18" t="s">
@@ -4709,7 +4709,7 @@
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="18"/>
       <c r="D15" s="18" t="s">
@@ -4719,7 +4719,7 @@
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="18"/>
       <c r="D16" s="18" t="s">
@@ -4729,7 +4729,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="18"/>
       <c r="D17" s="18" t="s">
@@ -4739,7 +4739,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="18"/>
       <c r="D18" s="18" t="s">
@@ -4749,7 +4749,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="18"/>
       <c r="D19" s="18" t="s">
@@ -4759,7 +4759,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="18"/>
       <c r="D20" s="18" t="s">
@@ -4769,7 +4769,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="18"/>
       <c r="D21" s="18" t="s">
@@ -4779,7 +4779,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="18"/>
       <c r="D22" s="18" t="s">
@@ -4789,7 +4789,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="18"/>
       <c r="D23" s="18" t="s">
@@ -4799,7 +4799,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="18"/>
       <c r="D24" s="18" t="s">
@@ -4809,7 +4809,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="18"/>
       <c r="D25" s="18" t="s">
@@ -4819,7 +4819,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="18"/>
       <c r="D26" s="18" t="s">
@@ -4829,13 +4829,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="3"/>
       <c r="D28" s="16" t="s">
@@ -4844,7 +4844,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="3"/>
       <c r="D29" s="16" t="s">

</xml_diff>

<commit_message>
In 1146 - Phase 2 setup (#640)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249C575E-F3E8-AC43-BCEA-AEC955C9E004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9744EA-75D7-584C-A8E9-2F36AC1D2D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1620" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="460" windowWidth="33600" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -226,9 +226,6 @@
     <t>NOT MAPPED</t>
   </si>
   <si>
-    <t>CASRECMIGRATION</t>
-  </si>
-  <si>
     <t>finance_invoice_ad</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>J-00-2-55-50</t>
+  </si>
+  <si>
+    <t>CASRECMIGRATION_P2</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>38</v>
@@ -760,15 +760,15 @@
         <v>54</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>38</v>
@@ -783,10 +783,10 @@
         <v>54</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -803,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="C13:O13"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -819,7 +819,7 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="15" width="11.5" customWidth="1"/>
     <col min="16" max="16" width="32.6640625" customWidth="1"/>
   </cols>
@@ -951,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="M5" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="12" t="s">
@@ -1064,7 +1064,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="12" t="s">
@@ -1158,7 +1158,7 @@
         <v>18</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>18</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>66</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="M15" s="13" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>18</v>
@@ -2671,9 +2671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B46E64-4858-2243-9F40-616107ECC251}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2821,7 +2821,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -2910,7 +2910,7 @@
         <v>58</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M7" s="2"/>
       <c r="O7" s="12" t="s">
@@ -2943,7 +2943,7 @@
         <v>58</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="12" t="s">
@@ -3037,7 +3037,7 @@
         <v>18</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3062,7 +3062,7 @@
         <v>18</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3087,7 +3087,7 @@
         <v>66</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -3137,7 +3137,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="M15" s="13" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>18</v>
@@ -4551,7 +4551,7 @@
   </sheetPr>
   <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="18"/>
       <c r="D5" s="18" t="s">
@@ -4619,7 +4619,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="18"/>
       <c r="D6" s="18" t="s">
@@ -4629,7 +4629,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="18"/>
       <c r="D7" s="18" t="s">
@@ -4639,7 +4639,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="18"/>
       <c r="D8" s="18" t="s">
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="18"/>
       <c r="D9" s="18" t="s">
@@ -4659,7 +4659,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="18"/>
       <c r="D10" s="18" t="s">
@@ -4669,7 +4669,7 @@
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="18"/>
       <c r="D11" s="18" t="s">
@@ -4679,7 +4679,7 @@
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="18"/>
       <c r="D12" s="18" t="s">
@@ -4689,7 +4689,7 @@
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="18"/>
       <c r="D13" s="18" t="s">
@@ -4699,7 +4699,7 @@
     </row>
     <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="18"/>
       <c r="D14" s="18" t="s">
@@ -4709,7 +4709,7 @@
     </row>
     <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="18"/>
       <c r="D15" s="18" t="s">
@@ -4719,7 +4719,7 @@
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="18"/>
       <c r="D16" s="18" t="s">
@@ -4729,7 +4729,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="18"/>
       <c r="D17" s="18" t="s">
@@ -4739,7 +4739,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="18"/>
       <c r="D18" s="18" t="s">
@@ -4749,7 +4749,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="18"/>
       <c r="D19" s="18" t="s">
@@ -4759,7 +4759,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="18"/>
       <c r="D20" s="18" t="s">
@@ -4769,7 +4769,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="18"/>
       <c r="D21" s="18" t="s">
@@ -4779,7 +4779,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="18"/>
       <c r="D22" s="18" t="s">
@@ -4789,7 +4789,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="18"/>
       <c r="D23" s="18" t="s">
@@ -4799,7 +4799,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="18"/>
       <c r="D24" s="18" t="s">
@@ -4809,7 +4809,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="18"/>
       <c r="D25" s="18" t="s">
@@ -4819,7 +4819,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="18"/>
       <c r="D26" s="18" t="s">
@@ -4829,13 +4829,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="3"/>
       <c r="D28" s="16" t="s">
@@ -4844,7 +4844,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="3"/>
       <c r="D29" s="16" t="s">

</xml_diff>